<commit_message>
commiting branch and bound files
</commit_message>
<xml_diff>
--- a/ComprehensiveTable.xlsx
+++ b/ComprehensiveTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanme\Documents\GitHub\TSP-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D1D194-53AA-4951-B214-0C280F46532E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA6467D1-5447-48BB-A7D2-E5816391FD51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4030CFC5-0913-4395-B916-0B7E2B5168A3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="26">
   <si>
     <t>Branch and Bound</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Mean Relative Error</t>
+  </si>
+  <si>
+    <t>Approximatio ratio</t>
   </si>
 </sst>
 </file>
@@ -132,7 +135,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -140,19 +143,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,41 +486,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9597F484-8077-4EA0-A22F-133B8DB563FE}">
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E2" t="s">
@@ -509,441 +530,560 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="D3" s="3">
-        <f t="shared" ref="D3:D15" si="0">(C3-E3)/E3</f>
-        <v>-1</v>
+      <c r="B3" s="3">
+        <v>42.25</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2003763</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
       </c>
       <c r="E3">
         <v>2003763</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="D4" s="3">
-        <f t="shared" si="0"/>
-        <v>-1</v>
+      <c r="B4" s="3">
+        <v>193.83</v>
+      </c>
+      <c r="C4" s="2">
+        <v>19023</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1.5222752585521</v>
       </c>
       <c r="E4">
         <v>7542</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="D5" s="3">
-        <f t="shared" si="0"/>
-        <v>-1</v>
+      <c r="B5" s="3">
+        <v>439.24</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2063922</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1.3098364251692101</v>
       </c>
       <c r="E5">
         <v>893536</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="D6" s="3">
-        <f t="shared" si="0"/>
-        <v>-1</v>
+      <c r="B6" s="3">
+        <v>582.77999999999895</v>
+      </c>
+      <c r="C6" s="2">
+        <v>196763</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2.7376859221548902</v>
       </c>
       <c r="E6">
         <v>52643</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="D7" s="3">
-        <f t="shared" si="0"/>
-        <v>-1</v>
+      <c r="B7" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C7" s="2">
+        <v>277952</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
       </c>
       <c r="E7">
         <v>277952</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="D8" s="3">
-        <f t="shared" si="0"/>
-        <v>-1</v>
+      <c r="B8" s="3">
+        <v>556.95000000000005</v>
+      </c>
+      <c r="C8" s="2">
+        <v>513066</v>
+      </c>
+      <c r="D8" s="4">
+        <v>4.1086417540400797</v>
       </c>
       <c r="E8">
         <v>100431</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="D9" s="3">
-        <f t="shared" si="0"/>
-        <v>-1</v>
+      <c r="B9" s="3">
+        <v>521.17999999999904</v>
+      </c>
+      <c r="C9" s="2">
+        <v>6964077</v>
+      </c>
+      <c r="D9" s="4">
+        <v>3.4783333118979298</v>
       </c>
       <c r="E9">
         <v>1555060</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="D10" s="3">
-        <f t="shared" si="0"/>
-        <v>-1</v>
+      <c r="B10" s="3">
+        <v>130.59</v>
+      </c>
+      <c r="C10" s="2">
+        <v>3487014</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1.4978950286572601</v>
       </c>
       <c r="E10">
         <v>1395981</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="D11" s="3">
-        <f t="shared" si="0"/>
-        <v>-1</v>
+      <c r="B11" s="3">
+        <v>314.26999999999902</v>
+      </c>
+      <c r="C11" s="2">
+        <v>6754456</v>
+      </c>
+      <c r="D11" s="4">
+        <v>9.3050038599199905</v>
       </c>
       <c r="E11">
         <v>655454</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="D12" s="3">
-        <f t="shared" si="0"/>
-        <v>-1</v>
+      <c r="B12" s="3">
+        <v>498.43999999999897</v>
+      </c>
+      <c r="C12" s="2">
+        <v>5417093</v>
+      </c>
+      <c r="D12" s="4">
+        <v>5.6861512522895596</v>
       </c>
       <c r="E12">
         <v>810196</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="D13" s="3">
-        <f t="shared" si="0"/>
-        <v>-1</v>
+      <c r="B13" s="3">
+        <v>380.13999999999902</v>
+      </c>
+      <c r="C13" s="2">
+        <v>8809227</v>
+      </c>
+      <c r="D13" s="4">
+        <v>6.4898775752433098</v>
       </c>
       <c r="E13">
         <v>1176151</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="D14" s="3">
-        <f t="shared" si="0"/>
-        <v>-1</v>
+      <c r="B14" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C14" s="2">
+        <v>62962</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0</v>
       </c>
       <c r="E14">
         <v>62962</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="D15" s="3">
-        <f t="shared" si="0"/>
-        <v>-1</v>
+      <c r="B15" s="3">
+        <v>375.12999999999897</v>
+      </c>
+      <c r="C15" s="2">
+        <v>640336</v>
+      </c>
+      <c r="D15" s="4">
+        <v>3.8251135944058001</v>
       </c>
       <c r="E15">
         <v>132709</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E18" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="F18" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="2">
-        <v>0</v>
-      </c>
-      <c r="C19">
+      <c r="B19" s="3">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2">
         <v>2415130</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="4">
         <v>0.20529723325562901</v>
       </c>
       <c r="E19">
         <v>2003763</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="F19" s="2">
+        <f>C19/E19</f>
+        <v>1.2052972332556295</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="2">
-        <v>0</v>
-      </c>
-      <c r="C20">
+      <c r="B20" s="3">
+        <v>0</v>
+      </c>
+      <c r="C20" s="2">
         <v>10303</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="4">
         <v>0.36608326703791999</v>
       </c>
       <c r="E20">
         <v>7542</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="F20" s="2">
+        <f t="shared" ref="F20:F31" si="0">C20/E20</f>
+        <v>1.366083267037921</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="2">
-        <v>0</v>
-      </c>
-      <c r="C21">
+      <c r="B21" s="3">
+        <v>0</v>
+      </c>
+      <c r="C21" s="2">
         <v>1094650</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="4">
         <v>0.22507654979765701</v>
       </c>
       <c r="E21">
         <v>893536</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="F21" s="2">
+        <f t="shared" si="0"/>
+        <v>1.2250765497976579</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="2">
-        <v>0</v>
-      </c>
-      <c r="C22">
+      <c r="B22" s="3">
+        <v>0</v>
+      </c>
+      <c r="C22" s="2">
         <v>61508</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="4">
         <v>0.168398457534714</v>
       </c>
       <c r="E22">
         <v>52643</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="F22" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1683984575347151</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="2">
-        <v>0</v>
-      </c>
-      <c r="C23">
+      <c r="B23" s="3">
+        <v>0</v>
+      </c>
+      <c r="C23" s="2">
         <v>315452</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="4">
         <v>0.134915381072991</v>
       </c>
       <c r="E23">
         <v>277952</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="F23" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1349153810729911</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="2">
-        <v>0</v>
-      </c>
-      <c r="C24">
+      <c r="B24" s="3">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2">
         <v>126189</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="4">
         <v>0.25647459449771398</v>
       </c>
       <c r="E24">
         <v>100431</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="F24" s="2">
+        <f t="shared" si="0"/>
+        <v>1.2564745944977149</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="2">
-        <v>0</v>
-      </c>
-      <c r="C25">
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
+      <c r="C25" s="2">
         <v>1884290</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="4">
         <v>0.211715303589572</v>
       </c>
       <c r="E25">
         <v>1555060</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="F25" s="2">
+        <f t="shared" si="0"/>
+        <v>1.211715303589572</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="2">
-        <v>0</v>
-      </c>
-      <c r="C26">
+      <c r="B26" s="3">
+        <v>0</v>
+      </c>
+      <c r="C26" s="2">
         <v>1722660</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="4">
         <v>0.23401392998901799</v>
       </c>
       <c r="E26">
         <v>1395981</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="F26" s="2">
+        <f t="shared" si="0"/>
+        <v>1.2340139299890185</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="2">
-        <v>0</v>
-      </c>
-      <c r="C27">
+      <c r="B27" s="3">
+        <v>0</v>
+      </c>
+      <c r="C27" s="2">
         <v>797872</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="4">
         <v>0.21728145682229399</v>
       </c>
       <c r="E27">
         <v>655454</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="F27" s="2">
+        <f t="shared" si="0"/>
+        <v>1.2172814568222943</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="2">
-        <v>0</v>
-      </c>
-      <c r="C28">
+      <c r="B28" s="3">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2">
         <v>1102580</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="4">
         <v>0.36088057704555399</v>
       </c>
       <c r="E28">
         <v>810196</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="F28" s="2">
+        <f t="shared" si="0"/>
+        <v>1.3608805770455543</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="2">
-        <v>0</v>
-      </c>
-      <c r="C29">
+      <c r="B29" s="3">
+        <v>0</v>
+      </c>
+      <c r="C29" s="2">
         <v>1686470</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="4">
         <v>0.43388901595118301</v>
       </c>
       <c r="E29">
         <v>1176151</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="F29" s="2">
+        <f t="shared" si="0"/>
+        <v>1.4338890159511832</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="2">
-        <v>0</v>
-      </c>
-      <c r="C30">
+      <c r="B30" s="3">
+        <v>0</v>
+      </c>
+      <c r="C30" s="2">
         <v>70143</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="4">
         <v>0.114052920809377</v>
       </c>
       <c r="E30">
         <v>62962</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="F30" s="2">
+        <f t="shared" si="0"/>
+        <v>1.114052920809377</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="2">
-        <v>0</v>
-      </c>
-      <c r="C31">
+      <c r="B31" s="3">
+        <v>0</v>
+      </c>
+      <c r="C31" s="2">
         <v>153757</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="4">
         <v>0.15860265694112599</v>
       </c>
       <c r="E31">
         <v>132709</v>
       </c>
+      <c r="F31" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1586026569411267</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="A34" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E34" t="s">
@@ -951,16 +1091,16 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="A35" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35" s="3">
         <v>9.9999999999999898E-3</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="5">
         <v>2066337.5</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="4">
         <v>3.12284935893117E-2</v>
       </c>
       <c r="E35">
@@ -968,16 +1108,16 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36" s="3">
         <v>0.20399999999999899</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="5">
         <v>8768.2000000000007</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="4">
         <v>0.16258286926544599</v>
       </c>
       <c r="E36">
@@ -985,16 +1125,16 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="A37" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37" s="3">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37" s="5">
         <v>979090.3</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="4">
         <v>9.5748016867815006E-2</v>
       </c>
       <c r="E37">
@@ -1002,16 +1142,16 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="A38" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38" s="3">
         <v>0.432999999999999</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38" s="5">
         <v>59926.5</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38" s="4">
         <v>0.13835647664456799</v>
       </c>
       <c r="E38">
@@ -1019,16 +1159,16 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="A39" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39" s="3">
         <v>2.2429999999999901</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C39" s="5">
         <v>558035.9</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="4">
         <v>7.6700293575869098E-3</v>
       </c>
       <c r="E39">
@@ -1036,16 +1176,16 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="A40" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40" s="3">
         <v>0.92200000000000004</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C40" s="5">
         <v>122477.6</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="4">
         <v>0.21951986936304499</v>
       </c>
       <c r="E40">
@@ -1053,16 +1193,16 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="A41" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41" s="3">
         <v>0.44399999999999901</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41" s="5">
         <v>1776027.5</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41" s="4">
         <v>0.142095803377361</v>
       </c>
       <c r="E41">
@@ -1070,16 +1210,16 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="A42" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42" s="3">
         <v>3.6999999999999901E-2</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="5">
         <v>1471237.1</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="4">
         <v>5.3909114808869098E-2</v>
       </c>
       <c r="E42">
@@ -1087,16 +1227,16 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="A43" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43" s="3">
         <v>18.942</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="5">
         <v>918843.4</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="4">
         <v>0.40184269224079699</v>
       </c>
       <c r="E43">
@@ -1104,16 +1244,16 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="A44" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44" s="3">
         <v>1.8660000000000001</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="5">
         <v>1080554.8</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="4">
         <v>0.33369555021254099</v>
       </c>
       <c r="E44">
@@ -1121,16 +1261,16 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="A45" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="3">
         <v>2.7779999999999898</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="5">
         <v>1573687.1</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="4">
         <v>0.33799750202142398</v>
       </c>
       <c r="E45">
@@ -1138,16 +1278,16 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="A46" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B46" s="2">
-        <v>0</v>
-      </c>
-      <c r="C46" s="1">
+      <c r="B46" s="3">
+        <v>0</v>
+      </c>
+      <c r="C46" s="5">
         <v>62962</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D46" s="4">
         <v>0</v>
       </c>
       <c r="E46">
@@ -1155,42 +1295,48 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+      <c r="A47" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47" s="3">
         <v>2.177</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="5">
         <v>162605.1</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D47" s="4">
         <v>0.225275603011099</v>
       </c>
       <c r="E47">
         <v>132709</v>
       </c>
     </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+    </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="1"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="A50" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E50" t="s">
@@ -1198,16 +1344,16 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+      <c r="A51" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51" s="3">
         <v>1.22599999999999</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" s="5">
         <v>2423113.2000000002</v>
       </c>
-      <c r="D51" s="3">
+      <c r="D51" s="4">
         <v>9.2813371641256893E-3</v>
       </c>
       <c r="E51">
@@ -1215,16 +1361,16 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+      <c r="A52" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B52" s="3">
         <v>7.6980000000000004</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="5">
         <v>8107.3</v>
       </c>
-      <c r="D52" s="3">
+      <c r="D52" s="4">
         <v>7.4953593211349701E-2</v>
       </c>
       <c r="E52">
@@ -1232,16 +1378,16 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+      <c r="A53" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53" s="3">
         <v>2.2329999999999899</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53" s="5">
         <v>923526.09999999905</v>
       </c>
-      <c r="D53" s="3">
+      <c r="D53" s="4">
         <v>3.3563393080972601E-2</v>
       </c>
       <c r="E53">
@@ -1249,16 +1395,16 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+      <c r="A54" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B54" s="3">
         <v>11.272</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C54" s="5">
         <v>53634.8</v>
       </c>
-      <c r="D54" s="3">
+      <c r="D54" s="4">
         <v>1.8840111695762E-2</v>
       </c>
       <c r="E54">
@@ -1266,16 +1412,16 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+      <c r="A55" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B55" s="3">
         <v>1.8379999999999901</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55" s="5">
         <v>278181.09999999899</v>
       </c>
-      <c r="D55" s="3">
+      <c r="D55" s="4">
         <v>8.2424303476859296E-4</v>
       </c>
       <c r="E55">
@@ -1283,16 +1429,16 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+      <c r="A56" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B56" s="3">
         <v>18.4559999999999</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56" s="5">
         <v>106975.5</v>
       </c>
-      <c r="D56" s="3">
+      <c r="D56" s="4">
         <v>6.5164142545628301E-2</v>
       </c>
       <c r="E56">
@@ -1300,16 +1446,16 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+      <c r="A57" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B57" s="3">
         <v>9.6679999999999993</v>
       </c>
-      <c r="C57" s="1">
+      <c r="C57" s="5">
         <v>1632378.6999999899</v>
       </c>
-      <c r="D57" s="3">
+      <c r="D57" s="4">
         <v>4.9720718171646097E-2</v>
       </c>
       <c r="E57">
@@ -1317,16 +1463,16 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+      <c r="A58" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B58" s="3">
         <v>1.69399999999999</v>
       </c>
-      <c r="C58" s="1">
+      <c r="C58" s="5">
         <v>1414553.1</v>
       </c>
-      <c r="D58" s="3">
+      <c r="D58" s="4">
         <v>1.3303977632933299E-2</v>
       </c>
       <c r="E58">
@@ -1334,16 +1480,16 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+      <c r="A59" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B59" s="3">
         <v>19.922999999999899</v>
       </c>
-      <c r="C59" s="1">
+      <c r="C59" s="5">
         <v>2062230.8999999899</v>
       </c>
-      <c r="D59" s="3">
+      <c r="D59" s="4">
         <v>2.1462633533398199</v>
       </c>
       <c r="E59">
@@ -1351,16 +1497,16 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+      <c r="A60" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B60" s="3">
         <v>19.032</v>
       </c>
-      <c r="C60" s="1">
+      <c r="C60" s="5">
         <v>895175.4</v>
       </c>
-      <c r="D60" s="3">
+      <c r="D60" s="4">
         <v>0.10488745933082801</v>
       </c>
       <c r="E60">
@@ -1368,16 +1514,16 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+      <c r="A61" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B61" s="2">
+      <c r="B61" s="3">
         <v>19.663</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61" s="5">
         <v>1325251.5</v>
       </c>
-      <c r="D61" s="3">
+      <c r="D61" s="4">
         <v>0.12676986203302101</v>
       </c>
       <c r="E61">
@@ -1385,16 +1531,16 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+      <c r="A62" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B62" s="3">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62" s="5">
         <v>62962</v>
       </c>
-      <c r="D62" s="3">
+      <c r="D62" s="4">
         <v>0</v>
       </c>
       <c r="E62">
@@ -1402,16 +1548,16 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+      <c r="A63" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B63" s="3">
         <v>19.611000000000001</v>
       </c>
-      <c r="C63" s="1">
+      <c r="C63" s="5">
         <v>148308.399999999</v>
       </c>
-      <c r="D63" s="3">
+      <c r="D63" s="4">
         <v>0.11754590871756999</v>
       </c>
       <c r="E63">
@@ -1419,10 +1565,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="A33:E33"/>
-    <mergeCell ref="A49:E49"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A49:D49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>